<commit_message>
Updated on 101018 10:10AM
</commit_message>
<xml_diff>
--- a/SMKRBoardDetails_210918.xlsx
+++ b/SMKRBoardDetails_210918.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="20730" windowHeight="9780"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="189">
   <si>
     <t>S.NO</t>
   </si>
@@ -798,6 +798,36 @@
       <t>24-08-18/30-09-18/30-10-18</t>
     </r>
   </si>
+  <si>
+    <t>Recharged on 03-09-18|Whenever the motor is switched to ON through APP, with in few seconds the motor is switched to OFF automatically(Replaced on 09-10-18 with SMKR0000086)Verify Row 32</t>
+  </si>
+  <si>
+    <t>SMKR0000086</t>
+  </si>
+  <si>
+    <t>SMKR0000086 Replaces SMKR0000078</t>
+  </si>
+  <si>
+    <t>MQTT(COM)</t>
+  </si>
+  <si>
+    <t>MQTT(NET)</t>
+  </si>
+  <si>
+    <r>
+      <t>6281559724/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>05-11-18</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -806,7 +836,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -837,8 +867,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -892,6 +935,12 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -921,7 +970,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -990,6 +1039,9 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -997,6 +1049,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1302,10 +1366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:AC32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1325,9 +1389,10 @@
     <col min="19" max="19" width="19" customWidth="1"/>
     <col min="20" max="20" width="52.5703125" customWidth="1"/>
     <col min="27" max="27" width="15.140625" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="3" customFormat="1">
+    <row r="1" spans="1:29" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1349,14 +1414,14 @@
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="25"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1366,12 +1431,12 @@
       <c r="N1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
       <c r="S1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1382,8 +1447,12 @@
       <c r="AA1" s="9" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" s="3" customFormat="1">
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" s="3" customFormat="1">
       <c r="B2" s="7"/>
       <c r="H2" s="3" t="s">
         <v>7</v>
@@ -1410,17 +1479,17 @@
         <v>18</v>
       </c>
       <c r="Z2" s="14"/>
-      <c r="AA2" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27">
+      <c r="AA2" s="24" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="N3" s="1"/>
       <c r="AA3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="13" customFormat="1">
+    <row r="4" spans="1:29" s="13" customFormat="1">
       <c r="A4" s="13">
         <v>1</v>
       </c>
@@ -1474,7 +1543,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="13" customFormat="1">
+    <row r="5" spans="1:29" s="13" customFormat="1">
       <c r="A5" s="13">
         <v>2</v>
       </c>
@@ -1530,10 +1599,10 @@
         <v>9441912299</v>
       </c>
       <c r="T5" s="13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" s="13" customFormat="1">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" s="13" customFormat="1">
       <c r="A6" s="13">
         <v>3</v>
       </c>
@@ -1595,7 +1664,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="13" customFormat="1">
+    <row r="7" spans="1:29" s="13" customFormat="1">
       <c r="A7" s="13">
         <v>4</v>
       </c>
@@ -1654,7 +1723,7 @@
         <v>9441565119</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="13" customFormat="1">
+    <row r="8" spans="1:29" s="13" customFormat="1">
       <c r="A8" s="13">
         <v>5</v>
       </c>
@@ -1707,7 +1776,7 @@
         <v>9182274792</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="1" customFormat="1">
+    <row r="9" spans="1:29" s="1" customFormat="1">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1760,7 +1829,7 @@
         <v>9959816503</v>
       </c>
     </row>
-    <row r="10" spans="1:27" s="1" customFormat="1">
+    <row r="10" spans="1:29" s="1" customFormat="1">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1822,7 +1891,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="1" customFormat="1">
+    <row r="11" spans="1:29" s="1" customFormat="1">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1881,7 +1950,7 @@
         <v>8332095555</v>
       </c>
     </row>
-    <row r="12" spans="1:27" s="1" customFormat="1">
+    <row r="12" spans="1:29" s="1" customFormat="1">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1931,7 +2000,7 @@
         <v>8328052306</v>
       </c>
     </row>
-    <row r="13" spans="1:27" s="1" customFormat="1">
+    <row r="13" spans="1:29" s="1" customFormat="1">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1990,7 +2059,7 @@
         <v>9866811840</v>
       </c>
     </row>
-    <row r="14" spans="1:27" s="10" customFormat="1">
+    <row r="14" spans="1:29" s="10" customFormat="1">
       <c r="A14" s="10">
         <v>11</v>
       </c>
@@ -2043,7 +2112,7 @@
         <v>7019668607</v>
       </c>
     </row>
-    <row r="15" spans="1:27" s="1" customFormat="1">
+    <row r="15" spans="1:29" s="1" customFormat="1">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -2087,7 +2156,7 @@
         <v>8985589895</v>
       </c>
     </row>
-    <row r="16" spans="1:27" s="1" customFormat="1">
+    <row r="16" spans="1:29" s="1" customFormat="1">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -2944,6 +3013,68 @@
       </c>
       <c r="T31" s="13" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" s="29" customFormat="1">
+      <c r="A32" s="29">
+        <v>29</v>
+      </c>
+      <c r="B32" s="30">
+        <v>43382</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I32" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="J32" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="K32" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="L32" s="29">
+        <v>12345</v>
+      </c>
+      <c r="M32" s="29">
+        <v>1234</v>
+      </c>
+      <c r="N32" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="O32" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="P32" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q32" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="R32" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="S32" s="29">
+        <v>9441912299</v>
+      </c>
+      <c r="T32" s="29" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>